<commit_message>
created run enviroment beta version. now with submission to stoomboot
need to test...
</commit_message>
<xml_diff>
--- a/runit/jobs.xlsx
+++ b/runit/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Gamma-ray_FastMC\runit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC313A1-03AB-4DD2-8AF9-C083EC43C929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA90D61-9EED-4D0C-8D31-E0466AEFF1D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8895" yWindow="3150" windowWidth="21600" windowHeight="11423" xr2:uid="{870F12B1-E48C-4968-876C-7F59D5E3880A}"/>
+    <workbookView xWindow="5153" yWindow="3533" windowWidth="21600" windowHeight="11422" xr2:uid="{870F12B1-E48C-4968-876C-7F59D5E3880A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>job_id</t>
   </si>
@@ -81,16 +81,49 @@
   </si>
   <si>
     <t>z_cryostat</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>/data/xenon/acolijn/mcdata/MC1</t>
+  </si>
+  <si>
+    <t>/data/xenon/acolijn/mcdata/MC2</t>
+  </si>
+  <si>
+    <t>/data/xenon/acolijn/mcdata/MC3</t>
+  </si>
+  <si>
+    <t>/data/xenon/acolijn/mcdata/MC4</t>
+  </si>
+  <si>
+    <t>/data/xenon/acolijn/mcdata/MC5</t>
+  </si>
+  <si>
+    <t>/data/xenon/acolijn/mcdata/MC6</t>
+  </si>
+  <si>
+    <t>/data/xenon/acolijn/mcdata/MC7</t>
+  </si>
+  <si>
+    <t>/data/xenon/acolijn/mcdata/MC8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -432,15 +465,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91896B0D-FA03-4CEB-A72D-CA18B2571B65}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="O2" sqref="O2:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="15" max="15" width="30.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +519,11 @@
       <c r="N1" t="s">
         <v>14</v>
       </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -513,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>42</v>
+        <v>12345</v>
       </c>
       <c r="K2">
         <v>65</v>
@@ -527,8 +566,11 @@
       <c r="N2">
         <v>134</v>
       </c>
+      <c r="O2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -557,7 +599,7 @@
         <v>2</v>
       </c>
       <c r="J3">
-        <v>43</v>
+        <v>12346</v>
       </c>
       <c r="K3">
         <v>65</v>
@@ -571,8 +613,11 @@
       <c r="N3">
         <v>134</v>
       </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -601,7 +646,7 @@
         <v>3</v>
       </c>
       <c r="J4">
-        <v>44</v>
+        <v>12347</v>
       </c>
       <c r="K4">
         <v>65</v>
@@ -615,8 +660,11 @@
       <c r="N4">
         <v>134</v>
       </c>
+      <c r="O4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -645,7 +693,7 @@
         <v>4</v>
       </c>
       <c r="J5">
-        <v>45</v>
+        <v>12348</v>
       </c>
       <c r="K5">
         <v>65</v>
@@ -659,8 +707,11 @@
       <c r="N5">
         <v>134</v>
       </c>
+      <c r="O5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -689,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="J6">
-        <v>46</v>
+        <v>12349</v>
       </c>
       <c r="K6">
         <v>65</v>
@@ -703,8 +754,11 @@
       <c r="N6">
         <v>134</v>
       </c>
+      <c r="O6" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -733,7 +787,7 @@
         <v>6</v>
       </c>
       <c r="J7">
-        <v>47</v>
+        <v>12350</v>
       </c>
       <c r="K7">
         <v>65</v>
@@ -747,8 +801,11 @@
       <c r="N7">
         <v>134</v>
       </c>
+      <c r="O7" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -777,7 +834,7 @@
         <v>7</v>
       </c>
       <c r="J8">
-        <v>48</v>
+        <v>12351</v>
       </c>
       <c r="K8">
         <v>65</v>
@@ -791,8 +848,11 @@
       <c r="N8">
         <v>134</v>
       </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -821,7 +881,7 @@
         <v>8</v>
       </c>
       <c r="J9">
-        <v>49</v>
+        <v>12352</v>
       </c>
       <c r="K9">
         <v>65</v>
@@ -835,8 +895,12 @@
       <c r="N9">
         <v>134</v>
       </c>
+      <c r="O9" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>